<commit_message>
fix bug using pyper library to run code R in python
</commit_message>
<xml_diff>
--- a/app_demo/output/M0102_example file_output.xlsx
+++ b/app_demo/output/M0102_example file_output.xlsx
@@ -479,7 +479,7 @@
         <v>226012.828125</v>
       </c>
       <c r="E2" t="n">
-        <v>160.8936901930977</v>
+        <v>187.4662394188178</v>
       </c>
     </row>
     <row r="3">
@@ -500,7 +500,7 @@
         <v>700359.375</v>
       </c>
       <c r="E3" t="n">
-        <v>38.43831399783159</v>
+        <v>44.78663001715602</v>
       </c>
     </row>
     <row r="4">
@@ -521,7 +521,7 @@
         <v>535785.0625</v>
       </c>
       <c r="E4" t="n">
-        <v>381.4139072154247</v>
+        <v>444.4066809698979</v>
       </c>
     </row>
     <row r="5">
@@ -542,7 +542,7 @@
         <v>3498388.5</v>
       </c>
       <c r="E5" t="n">
-        <v>192.0045057573521</v>
+        <v>223.7151910842536</v>
       </c>
     </row>
     <row r="6">
@@ -563,7 +563,7 @@
         <v>81616.8046875</v>
       </c>
       <c r="E6" t="n">
-        <v>26.17032827868239</v>
+        <v>30.4925135402917</v>
       </c>
     </row>
     <row r="7">
@@ -584,7 +584,7 @@
         <v>94598.234375</v>
       </c>
       <c r="E7" t="n">
-        <v>5.191901138678575</v>
+        <v>6.049374470398623</v>
       </c>
     </row>
     <row r="8">
@@ -605,7 +605,7 @@
         <v>110015.2890625</v>
       </c>
       <c r="E8" t="n">
-        <v>78.31752729157601</v>
+        <v>91.25213241309717</v>
       </c>
     </row>
     <row r="9">
@@ -626,7 +626,7 @@
         <v>698144.6875</v>
       </c>
       <c r="E9" t="n">
-        <v>223.8592374186804</v>
+        <v>260.8309210117467</v>
       </c>
     </row>
     <row r="10">
@@ -647,7 +647,7 @@
         <v>512776.78125</v>
       </c>
       <c r="E10" t="n">
-        <v>164.421245727277</v>
+        <v>191.5763917159027</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
         <v>107556.9296875</v>
       </c>
       <c r="E11" t="n">
-        <v>34.48799753122576</v>
+        <v>40.18389530692563</v>
       </c>
     </row>
     <row r="12">
@@ -689,7 +689,7 @@
         <v>2533992.75</v>
       </c>
       <c r="E12" t="n">
-        <v>812.5216660614707</v>
+        <v>946.7144485283916</v>
       </c>
     </row>
     <row r="13">
@@ -710,7 +710,7 @@
         <v>89390.890625</v>
       </c>
       <c r="E13" t="n">
-        <v>28.66307939568639</v>
+        <v>33.39695732022464</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +782,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>160.8936901930977</t>
+          <t>187.4662394188178</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.07407407407407407</t>
+          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.0740740740740741</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -838,7 +838,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>38.438313997831585</t>
+          <t>44.78663001715602</t>
         </is>
       </c>
     </row>
@@ -857,7 +857,7 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.061224489795918366</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.0612244897959184</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -894,7 +894,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>381.41390721542473</t>
+          <t>444.40668096989793</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.058823529411764705</t>
+          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.0588235294117647</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -950,7 +950,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>192.00450575735215</t>
+          <t>223.7151910842536</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.05128205128205128</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.0512820512820513</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>26.17032827868239</t>
+          <t>30.492513540291704</t>
         </is>
       </c>
     </row>
@@ -1025,7 +1025,7 @@
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.038461538461538464</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.0384615384615385</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>5.191901138678575</t>
+          <t>6.049374470398623</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.028169014084507043</t>
+          <t>Best Match: C(C(F)(F)F)(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F with Similarity: 0.028169014084507</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>78.31752729157601</t>
+          <t>91.25213241309717</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.05102040816326531</t>
+          <t>Best Match: C(C(C(C(F)(F)Cl)(F)F)(F)F)(C(C(OC(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(F)F)(F)F with Similarity: 0.0510204081632653</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>223.8592374186804</t>
+          <t>260.8309210117467</t>
         </is>
       </c>
     </row>
@@ -1193,7 +1193,7 @@
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.044444444444444446</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.0444444444444444</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>164.42124572727695</t>
+          <t>191.57639171590267</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.025974025974025976</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.025974025974026</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>34.48799753122576</t>
+          <t>40.18389530692563</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.022222222222222223</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.0222222222222222</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>812.5216660614707</t>
+          <t>946.7144485283916</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>28.663079395686392</t>
+          <t>33.39695732022464</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.025974025974025976</t>
+          <t>Best Match: C(C(C(C(F)(F)S(=O)(=O)O)(F)F)(F)F)(C(C(F)(F)F)(F)F)(F)F with Similarity: 0.025974025974026</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>

</xml_diff>